<commit_message>
ML project 2 review seed
</commit_message>
<xml_diff>
--- a/ML_PR/Pattern Rec/Project 1/Proj1DataSet.xlsx
+++ b/ML_PR/Pattern Rec/Project 1/Proj1DataSet.xlsx
@@ -1,16 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silas\Documents\Python_Projects\ML_PR\Pattern Rec\Project 1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA8705E-6F1D-428B-814E-E64D4BCE903D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -44,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -59,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -67,36 +74,347 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E151"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:E151"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" customWidth="true"/>
-    <col min="2" max="2" width="7.85546875" customWidth="true"/>
-    <col min="3" max="3" width="7.85546875" customWidth="true"/>
-    <col min="4" max="4" width="7.85546875" customWidth="true"/>
-    <col min="5" max="5" width="9.85546875" customWidth="true"/>
+    <col min="1" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -113,7 +431,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>5.0999999999999996</v>
       </c>
@@ -121,16 +439,16 @@
         <v>3.5</v>
       </c>
       <c r="C2">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D2">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>4.9000000000000004</v>
       </c>
@@ -138,205 +456,205 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D3">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4">
-        <v>4.7000000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="B4">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C4">
         <v>1.3</v>
       </c>
       <c r="D4">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4.5999999999999996</v>
       </c>
       <c r="B5">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C5">
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="C6">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D6">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="B7">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="C7">
         <v>1.7</v>
       </c>
       <c r="D7">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>4.5999999999999996</v>
       </c>
       <c r="B8">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C8">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D8">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C9">
         <v>1.5</v>
       </c>
       <c r="D9">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>4.4000000000000004</v>
       </c>
       <c r="B10">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C10">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D10">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>4.9000000000000004</v>
       </c>
       <c r="B11">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C11">
         <v>1.5</v>
       </c>
       <c r="D11">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="B12">
-        <v>3.7000000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="C12">
         <v>1.5</v>
       </c>
       <c r="D12">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="B13">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C13">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D13">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D14">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15">
-        <v>4.2999999999999998</v>
+        <v>4.3</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -345,15 +663,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D15">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5">
       <c r="A16">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -362,15 +680,15 @@
         <v>1.2</v>
       </c>
       <c r="D16">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5">
       <c r="A17">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="B17">
         <v>4.4000000000000004</v>
@@ -379,30 +697,30 @@
         <v>1.5</v>
       </c>
       <c r="D17">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5">
       <c r="A18">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="B18">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="C18">
         <v>1.3</v>
       </c>
       <c r="D18">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>5.0999999999999996</v>
       </c>
@@ -410,106 +728,106 @@
         <v>3.5</v>
       </c>
       <c r="C19">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D19">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5">
       <c r="A20">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="B20">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="C20">
         <v>1.7</v>
       </c>
       <c r="D20">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>5.0999999999999996</v>
       </c>
       <c r="B21">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="C21">
         <v>1.5</v>
       </c>
       <c r="D21">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5">
       <c r="A22">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="B22">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C22">
         <v>1.7</v>
       </c>
       <c r="D22">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>5.0999999999999996</v>
       </c>
       <c r="B23">
-        <v>3.7000000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="C23">
         <v>1.5</v>
       </c>
       <c r="D23">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>4.5999999999999996</v>
       </c>
       <c r="B24">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>5.0999999999999996</v>
       </c>
       <c r="B25">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="C25">
         <v>1.7</v>
@@ -521,24 +839,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5">
       <c r="A26">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="B26">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C26">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D26">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>5</v>
       </c>
@@ -546,35 +864,35 @@
         <v>3</v>
       </c>
       <c r="C27">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D27">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>5</v>
       </c>
       <c r="B28">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C28">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D28">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5">
       <c r="A29">
-        <v>5.2000000000000002</v>
+        <v>5.2</v>
       </c>
       <c r="B29">
         <v>3.5</v>
@@ -583,83 +901,83 @@
         <v>1.5</v>
       </c>
       <c r="D29">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5">
       <c r="A30">
-        <v>5.2000000000000002</v>
+        <v>5.2</v>
       </c>
       <c r="B30">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C30">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D30">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5">
       <c r="A31">
-        <v>4.7000000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="B31">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C31">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D31">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5">
       <c r="A32">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="B32">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C32">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D32">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5">
       <c r="A33">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="B33">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C33">
         <v>1.5</v>
       </c>
       <c r="D33">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5">
       <c r="A34">
-        <v>5.2000000000000002</v>
+        <v>5.2</v>
       </c>
       <c r="B34">
         <v>4.0999999999999996</v>
@@ -668,64 +986,64 @@
         <v>1.5</v>
       </c>
       <c r="D34">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>5.5</v>
       </c>
       <c r="B35">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="C35">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D35">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>4.9000000000000004</v>
       </c>
       <c r="B36">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C36">
         <v>1.5</v>
       </c>
       <c r="D36">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>5</v>
       </c>
       <c r="B37">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C37">
         <v>1.2</v>
       </c>
       <c r="D37">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>5.5</v>
       </c>
@@ -736,30 +1054,30 @@
         <v>1.3</v>
       </c>
       <c r="D38">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>4.9000000000000004</v>
       </c>
       <c r="B39">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="C39">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D39">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>4.4000000000000004</v>
       </c>
@@ -770,30 +1088,30 @@
         <v>1.3</v>
       </c>
       <c r="D40">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>5.0999999999999996</v>
       </c>
       <c r="B41">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C41">
         <v>1.5</v>
       </c>
       <c r="D41">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>5</v>
       </c>
@@ -804,13 +1122,13 @@
         <v>1.3</v>
       </c>
       <c r="D42">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>4.5</v>
       </c>
@@ -821,30 +1139,30 @@
         <v>1.3</v>
       </c>
       <c r="D43">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>4.4000000000000004</v>
       </c>
       <c r="B44">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C44">
         <v>1.3</v>
       </c>
       <c r="D44">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>5</v>
       </c>
@@ -852,140 +1170,140 @@
         <v>3.5</v>
       </c>
       <c r="C45">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D45">
-        <v>0.59999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>5.0999999999999996</v>
       </c>
       <c r="B46">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="C46">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D46">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:5">
       <c r="A47">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="B47">
         <v>3</v>
       </c>
       <c r="C47">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D47">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>5.0999999999999996</v>
       </c>
       <c r="B48">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="C48">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D48">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>4.5999999999999996</v>
       </c>
       <c r="B49">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C49">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D49">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:5">
       <c r="A50">
-        <v>5.2999999999999998</v>
+        <v>5.3</v>
       </c>
       <c r="B50">
-        <v>3.7000000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="C50">
         <v>1.5</v>
       </c>
       <c r="D50">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>5</v>
       </c>
       <c r="B51">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="C51">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D51">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>7</v>
       </c>
       <c r="B52">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C52">
-        <v>4.7000000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="D52">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:5">
       <c r="A53">
-        <v>6.4000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="B53">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C53">
         <v>4.5</v>
@@ -997,12 +1315,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:5">
       <c r="A54">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="B54">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C54">
         <v>4.9000000000000004</v>
@@ -1014,7 +1332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>5.5</v>
       </c>
@@ -1031,12 +1349,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>6.5</v>
       </c>
       <c r="B56">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C56">
         <v>4.5999999999999996</v>
@@ -1048,12 +1366,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:5">
       <c r="A57">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="B57">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C57">
         <v>4.5</v>
@@ -1065,32 +1383,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:5">
       <c r="A58">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="B58">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="C58">
-        <v>4.7000000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="D58">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>4.9000000000000004</v>
       </c>
       <c r="B59">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="C59">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -1099,12 +1417,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:5">
       <c r="A60">
-        <v>6.5999999999999996</v>
+        <v>6.6</v>
       </c>
       <c r="B60">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C60">
         <v>4.5999999999999996</v>
@@ -1116,24 +1434,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:5">
       <c r="A61">
-        <v>5.2000000000000002</v>
+        <v>5.2</v>
       </c>
       <c r="B61">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C61">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="D61">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>5</v>
       </c>
@@ -1150,15 +1468,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:5">
       <c r="A63">
-        <v>5.9000000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="B63">
         <v>3</v>
       </c>
       <c r="C63">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="D63">
         <v>1.5</v>
@@ -1167,7 +1485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>6</v>
       </c>
@@ -1184,32 +1502,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:5">
       <c r="A65">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="B65">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C65">
-        <v>4.7000000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="D65">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:5">
       <c r="A66">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="B66">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C66">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="D66">
         <v>1.3</v>
@@ -1218,26 +1536,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:5">
       <c r="A67">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="B67">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C67">
         <v>4.4000000000000004</v>
       </c>
       <c r="D67">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:5">
       <c r="A68">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="B68">
         <v>3</v>
@@ -1252,12 +1570,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:5">
       <c r="A69">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="B69">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C69">
         <v>4.0999999999999996</v>
@@ -1269,9 +1587,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:5">
       <c r="A70">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="B70">
         <v>2.2000000000000002</v>
@@ -1286,15 +1604,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:5">
       <c r="A71">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="B71">
         <v>2.5</v>
       </c>
       <c r="C71">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="D71">
         <v>1.1000000000000001</v>
@@ -1303,15 +1621,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:5">
       <c r="A72">
-        <v>5.9000000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="B72">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C72">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="D72">
         <v>1.8</v>
@@ -1320,12 +1638,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:5">
       <c r="A73">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="B73">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C73">
         <v>4</v>
@@ -1337,9 +1655,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:5">
       <c r="A74">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="B74">
         <v>2.5</v>
@@ -1354,15 +1672,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:5">
       <c r="A75">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="B75">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C75">
-        <v>4.7000000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="D75">
         <v>1.2</v>
@@ -1371,15 +1689,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:5">
       <c r="A76">
-        <v>6.4000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="B76">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C76">
-        <v>4.2999999999999998</v>
+        <v>4.3</v>
       </c>
       <c r="D76">
         <v>1.3</v>
@@ -1388,9 +1706,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:5">
       <c r="A77">
-        <v>6.5999999999999996</v>
+        <v>6.6</v>
       </c>
       <c r="B77">
         <v>3</v>
@@ -1399,32 +1717,32 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D77">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:5">
       <c r="A78">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="B78">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C78">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="D78">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:5">
       <c r="A79">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="B79">
         <v>3</v>
@@ -1439,12 +1757,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>6</v>
       </c>
       <c r="B80">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C80">
         <v>4.5</v>
@@ -1456,12 +1774,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:5">
       <c r="A81">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="B81">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="C81">
         <v>3.5</v>
@@ -1473,15 +1791,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>5.5</v>
       </c>
       <c r="B82">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="C82">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="D82">
         <v>1.1000000000000001</v>
@@ -1490,15 +1808,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>5.5</v>
       </c>
       <c r="B83">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="C83">
-        <v>3.7000000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -1507,15 +1825,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:5">
       <c r="A84">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="B84">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C84">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="D84">
         <v>1.2</v>
@@ -1524,26 +1842,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>6</v>
       </c>
       <c r="B85">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C85">
         <v>5.0999999999999996</v>
       </c>
       <c r="D85">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:5">
       <c r="A86">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="B86">
         <v>3</v>
@@ -1558,32 +1876,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>6</v>
       </c>
       <c r="B87">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C87">
         <v>4.5</v>
       </c>
       <c r="D87">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:5">
       <c r="A88">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="B88">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C88">
-        <v>4.7000000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="D88">
         <v>1.5</v>
@@ -1592,9 +1910,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:5">
       <c r="A89">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="B89">
         <v>2.2999999999999998</v>
@@ -1609,9 +1927,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:5">
       <c r="A90">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -1626,7 +1944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>5.5</v>
       </c>
@@ -1643,12 +1961,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>5.5</v>
       </c>
       <c r="B92">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="C92">
         <v>4.4000000000000004</v>
@@ -1660,9 +1978,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:5">
       <c r="A93">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="B93">
         <v>3</v>
@@ -1671,18 +1989,18 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D93">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:5">
       <c r="A94">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="B94">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="C94">
         <v>4</v>
@@ -1694,7 +2012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>5</v>
       </c>
@@ -1702,7 +2020,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C95">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -1711,15 +2029,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:5">
       <c r="A96">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="B96">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C96">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="D96">
         <v>1.3</v>
@@ -1728,15 +2046,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:5">
       <c r="A97">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="B97">
         <v>3</v>
       </c>
       <c r="C97">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="D97">
         <v>1.2</v>
@@ -1745,15 +2063,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:5">
       <c r="A98">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="B98">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C98">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="D98">
         <v>1.3</v>
@@ -1762,15 +2080,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:5">
       <c r="A99">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="B99">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C99">
-        <v>4.2999999999999998</v>
+        <v>4.3</v>
       </c>
       <c r="D99">
         <v>1.3</v>
@@ -1779,7 +2097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>5.0999999999999996</v>
       </c>
@@ -1796,12 +2114,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:5">
       <c r="A101">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="B101">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C101">
         <v>4.0999999999999996</v>
@@ -1813,12 +2131,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:5">
       <c r="A102">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="B102">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="C102">
         <v>6</v>
@@ -1830,49 +2148,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:5">
       <c r="A103">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="B103">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C103">
         <v>5.0999999999999996</v>
       </c>
       <c r="D103">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:5">
       <c r="A104">
-        <v>7.0999999999999996</v>
+        <v>7.1</v>
       </c>
       <c r="B104">
         <v>3</v>
       </c>
       <c r="C104">
-        <v>5.9000000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="D104">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:5">
       <c r="A105">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="B105">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C105">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="D105">
         <v>1.8</v>
@@ -1881,7 +2199,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>6.5</v>
       </c>
@@ -1889,7 +2207,7 @@
         <v>3</v>
       </c>
       <c r="C106">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="D106">
         <v>2.2000000000000002</v>
@@ -1898,24 +2216,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:5">
       <c r="A107">
-        <v>7.5999999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="B107">
         <v>3</v>
       </c>
       <c r="C107">
-        <v>6.5999999999999996</v>
+        <v>6.6</v>
       </c>
       <c r="D107">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>4.9000000000000004</v>
       </c>
@@ -1932,15 +2250,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:5">
       <c r="A109">
-        <v>7.2999999999999998</v>
+        <v>7.3</v>
       </c>
       <c r="B109">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="C109">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="D109">
         <v>1.8</v>
@@ -1949,15 +2267,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:5">
       <c r="A110">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="B110">
         <v>2.5</v>
       </c>
       <c r="C110">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="D110">
         <v>1.8</v>
@@ -1966,15 +2284,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:5">
       <c r="A111">
-        <v>7.2000000000000002</v>
+        <v>7.2</v>
       </c>
       <c r="B111">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="C111">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="D111">
         <v>2.5</v>
@@ -1983,12 +2301,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>6.5</v>
       </c>
       <c r="B112">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C112">
         <v>5.0999999999999996</v>
@@ -2000,26 +2318,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:5">
       <c r="A113">
-        <v>6.4000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="B113">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C113">
-        <v>5.2999999999999998</v>
+        <v>5.3</v>
       </c>
       <c r="D113">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:5">
       <c r="A114">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -2028,15 +2346,15 @@
         <v>5.5</v>
       </c>
       <c r="D114">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:5">
       <c r="A115">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="B115">
         <v>2.5</v>
@@ -2051,32 +2369,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:5">
       <c r="A116">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="B116">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C116">
         <v>5.0999999999999996</v>
       </c>
       <c r="D116">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:5">
       <c r="A117">
-        <v>6.4000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="B117">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C117">
-        <v>5.2999999999999998</v>
+        <v>5.3</v>
       </c>
       <c r="D117">
         <v>2.2999999999999998</v>
@@ -2085,7 +2403,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:5">
       <c r="A118">
         <v>6.5</v>
       </c>
@@ -2102,15 +2420,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:5">
       <c r="A119">
-        <v>7.7000000000000002</v>
+        <v>7.7</v>
       </c>
       <c r="B119">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="C119">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="D119">
         <v>2.2000000000000002</v>
@@ -2119,15 +2437,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:5">
       <c r="A120">
-        <v>7.7000000000000002</v>
+        <v>7.7</v>
       </c>
       <c r="B120">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="C120">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="D120">
         <v>2.2999999999999998</v>
@@ -2136,7 +2454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:5">
       <c r="A121">
         <v>6</v>
       </c>
@@ -2153,15 +2471,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:5">
       <c r="A122">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="B122">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C122">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="D122">
         <v>2.2999999999999998</v>
@@ -2170,12 +2488,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:5">
       <c r="A123">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="B123">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C123">
         <v>4.9000000000000004</v>
@@ -2187,15 +2505,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:5">
       <c r="A124">
-        <v>7.7000000000000002</v>
+        <v>7.7</v>
       </c>
       <c r="B124">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C124">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="D124">
         <v>2</v>
@@ -2204,12 +2522,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:5">
       <c r="A125">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="B125">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C125">
         <v>4.9000000000000004</v>
@@ -2221,29 +2539,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:5">
       <c r="A126">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="B126">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="C126">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="D126">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:5">
       <c r="A127">
-        <v>7.2000000000000002</v>
+        <v>7.2</v>
       </c>
       <c r="B127">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C127">
         <v>6</v>
@@ -2255,15 +2573,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:5">
       <c r="A128">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="B128">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C128">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="D128">
         <v>1.8</v>
@@ -2272,9 +2590,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:5">
       <c r="A129">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="B129">
         <v>3</v>
@@ -2289,66 +2607,66 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:5">
       <c r="A130">
-        <v>6.4000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="B130">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C130">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="D130">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:5">
       <c r="A131">
-        <v>7.2000000000000002</v>
+        <v>7.2</v>
       </c>
       <c r="B131">
         <v>3</v>
       </c>
       <c r="C131">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="D131">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:5">
       <c r="A132">
-        <v>7.4000000000000004</v>
+        <v>7.4</v>
       </c>
       <c r="B132">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C132">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="D132">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:5">
       <c r="A133">
-        <v>7.9000000000000004</v>
+        <v>7.9</v>
       </c>
       <c r="B133">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="C133">
-        <v>6.4000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="D133">
         <v>2</v>
@@ -2357,15 +2675,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:5">
       <c r="A134">
-        <v>6.4000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="B134">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C134">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="D134">
         <v>2.2000000000000002</v>
@@ -2374,12 +2692,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:5">
       <c r="A135">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="B135">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C135">
         <v>5.0999999999999996</v>
@@ -2391,32 +2709,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:5">
       <c r="A136">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="B136">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="C136">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="D136">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:5">
       <c r="A137">
-        <v>7.7000000000000002</v>
+        <v>7.7</v>
       </c>
       <c r="B137">
         <v>3</v>
       </c>
       <c r="C137">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="D137">
         <v>2.2999999999999998</v>
@@ -2425,29 +2743,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:5">
       <c r="A138">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="B138">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C138">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="D138">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:5">
       <c r="A139">
-        <v>6.4000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="B139">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C139">
         <v>5.5</v>
@@ -2459,7 +2777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:5">
       <c r="A140">
         <v>6</v>
       </c>
@@ -2467,7 +2785,7 @@
         <v>3</v>
       </c>
       <c r="C140">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="D140">
         <v>1.8</v>
@@ -2476,46 +2794,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:5">
       <c r="A141">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="B141">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C141">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="D141">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:5">
       <c r="A142">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="B142">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C142">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="D142">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:5">
       <c r="A143">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="B143">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="C143">
         <v>5.0999999999999996</v>
@@ -2527,32 +2845,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:5">
       <c r="A144">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="B144">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C144">
         <v>5.0999999999999996</v>
       </c>
       <c r="D144">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:5">
       <c r="A145">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="B145">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="C145">
-        <v>5.9000000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="D145">
         <v>2.2999999999999998</v>
@@ -2561,15 +2879,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:5">
       <c r="A146">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="B146">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="C146">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="D146">
         <v>2.5</v>
@@ -2578,15 +2896,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:5">
       <c r="A147">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="B147">
         <v>3</v>
       </c>
       <c r="C147">
-        <v>5.2000000000000002</v>
+        <v>5.2</v>
       </c>
       <c r="D147">
         <v>2.2999999999999998</v>
@@ -2595,9 +2913,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:5">
       <c r="A148">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="B148">
         <v>2.5</v>
@@ -2606,13 +2924,13 @@
         <v>5</v>
       </c>
       <c r="D148">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:5">
       <c r="A149">
         <v>6.5</v>
       </c>
@@ -2620,7 +2938,7 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>5.2000000000000002</v>
+        <v>5.2</v>
       </c>
       <c r="D149">
         <v>2</v>
@@ -2629,15 +2947,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:5">
       <c r="A150">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="B150">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="C150">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="D150">
         <v>2.2999999999999998</v>
@@ -2646,9 +2964,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:5">
       <c r="A151">
-        <v>5.9000000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="B151">
         <v>3</v>
@@ -2664,21 +2982,30 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>